<commit_message>
chefs warehouse, barons, bakers are working
</commit_message>
<xml_diff>
--- a/spec/lib/product_import/test_data/chefs_warehouse.xlsx
+++ b/spec/lib/product_import/test_data/chefs_warehouse.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26101"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colthorp/Repositories/localorbit/web/spec/lib/product_import/test_data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="2900" windowWidth="20740" windowHeight="11760"/>
+    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="20460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -869,10 +874,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -895,13 +916,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="11">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1222,11 +1263,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37.5" customWidth="1"/>
     <col min="2" max="2" width="10.1640625" customWidth="1"/>
@@ -1242,7 +1283,7 @@
     <col min="14" max="16" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1265,7 +1306,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -1288,7 +1329,7 @@
         <v>222.65</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1311,7 +1352,7 @@
         <v>22.34</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1334,7 +1375,7 @@
         <v>25.25</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -1357,7 +1398,7 @@
         <v>27.29</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>117</v>
       </c>
@@ -1380,7 +1421,7 @@
         <v>20.98</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>117</v>
       </c>
@@ -1403,7 +1444,7 @@
         <v>37.31</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>117</v>
       </c>
@@ -1426,7 +1467,7 @@
         <v>24.57</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>117</v>
       </c>
@@ -1449,7 +1490,7 @@
         <v>35.29</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>117</v>
       </c>
@@ -1472,7 +1513,7 @@
         <v>29.05</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>117</v>
       </c>
@@ -1495,7 +1536,7 @@
         <v>31.71</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>117</v>
       </c>
@@ -1518,7 +1559,7 @@
         <v>39.49</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>117</v>
       </c>
@@ -1541,7 +1582,7 @@
         <v>67.27</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>117</v>
       </c>
@@ -1564,7 +1605,7 @@
         <v>28.26</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>117</v>
       </c>
@@ -1587,7 +1628,7 @@
         <v>30.55</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>117</v>
       </c>
@@ -1610,7 +1651,7 @@
         <v>29.19</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>270</v>
       </c>
@@ -1633,7 +1674,7 @@
         <v>62.79</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>253</v>
       </c>
@@ -1656,7 +1697,7 @@
         <v>22.98</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>253</v>
       </c>
@@ -1679,7 +1720,7 @@
         <v>22.98</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>253</v>
       </c>
@@ -1702,7 +1743,7 @@
         <v>22.98</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1725,7 +1766,7 @@
         <v>13.17</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1748,7 +1789,7 @@
         <v>7.94</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>90</v>
       </c>
@@ -1771,7 +1812,7 @@
         <v>10.65</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>90</v>
       </c>
@@ -1794,7 +1835,7 @@
         <v>21.25</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>90</v>
       </c>
@@ -1817,7 +1858,7 @@
         <v>22.98</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>195</v>
       </c>
@@ -1840,7 +1881,7 @@
         <v>6.08</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>199</v>
       </c>
@@ -1863,7 +1904,7 @@
         <v>14.51</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>127</v>
       </c>
@@ -1886,7 +1927,7 @@
         <v>6.82</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>127</v>
       </c>
@@ -1909,7 +1950,7 @@
         <v>9.2200000000000006</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>141</v>
       </c>
@@ -1932,7 +1973,7 @@
         <v>254.5</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>141</v>
       </c>
@@ -1955,7 +1996,7 @@
         <v>15.15</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>153</v>
       </c>
@@ -1978,7 +2019,7 @@
         <v>5.49</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>161</v>
       </c>
@@ -2001,7 +2042,7 @@
         <v>4.78</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>149</v>
       </c>
@@ -2024,7 +2065,7 @@
         <v>3.18</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>187</v>
       </c>
@@ -2047,7 +2088,7 @@
         <v>11.41</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>157</v>
       </c>
@@ -2070,7 +2111,7 @@
         <v>7.08</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>191</v>
       </c>
@@ -2093,7 +2134,7 @@
         <v>13.75</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>71</v>
       </c>
@@ -2116,7 +2157,7 @@
         <v>9.65</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>168</v>
       </c>
@@ -2139,7 +2180,7 @@
         <v>16.97</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -2162,7 +2203,7 @@
         <v>100.01</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>145</v>
       </c>
@@ -2185,7 +2226,7 @@
         <v>52.89</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>145</v>
       </c>
@@ -2208,7 +2249,7 @@
         <v>49.57</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>134</v>
       </c>
@@ -2231,7 +2272,7 @@
         <v>55.97</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>138</v>
       </c>
@@ -2254,7 +2295,7 @@
         <v>46.94</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>138</v>
       </c>
@@ -2277,7 +2318,7 @@
         <v>41.42</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>75</v>
       </c>
@@ -2300,7 +2341,7 @@
         <v>10.45</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>75</v>
       </c>
@@ -2323,7 +2364,7 @@
         <v>8.43</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>220</v>
       </c>
@@ -2346,7 +2387,7 @@
         <v>22.73</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>232</v>
       </c>
@@ -2369,7 +2410,7 @@
         <v>45.11</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>22</v>
       </c>
@@ -2392,7 +2433,7 @@
         <v>16.760000000000002</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>22</v>
       </c>
@@ -2415,7 +2456,7 @@
         <v>10.61</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>30</v>
       </c>
@@ -2438,7 +2479,7 @@
         <v>7.77</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -2461,7 +2502,7 @@
         <v>131.22999999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>104</v>
       </c>
@@ -2484,7 +2525,7 @@
         <v>32.049999999999997</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>100</v>
       </c>
@@ -2507,7 +2548,7 @@
         <v>34.42</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>111</v>
       </c>
@@ -2530,7 +2571,7 @@
         <v>71.180000000000007</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>111</v>
       </c>
@@ -2553,7 +2594,7 @@
         <v>63.31</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>111</v>
       </c>
@@ -2576,7 +2617,7 @@
         <v>49.96</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>111</v>
       </c>
@@ -2599,7 +2640,7 @@
         <v>39.5</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>111</v>
       </c>
@@ -2622,7 +2663,7 @@
         <v>62.44</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>111</v>
       </c>
@@ -2645,7 +2686,7 @@
         <v>23.54</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>111</v>
       </c>
@@ -2668,7 +2709,7 @@
         <v>68.72</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>111</v>
       </c>
@@ -2691,7 +2732,7 @@
         <v>32.08</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>12</v>
       </c>
@@ -2714,7 +2755,7 @@
         <v>38.75</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>26</v>
       </c>
@@ -2737,7 +2778,7 @@
         <v>10.33</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>17</v>
       </c>
@@ -2760,7 +2801,7 @@
         <v>15.78</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -2783,7 +2824,7 @@
         <v>40.98</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>243</v>
       </c>
@@ -2806,7 +2847,7 @@
         <v>34.82</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>63</v>
       </c>
@@ -2829,7 +2870,7 @@
         <v>34.229999999999997</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>34</v>
       </c>
@@ -2852,7 +2893,7 @@
         <v>113.07</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>34</v>
       </c>
@@ -2875,7 +2916,7 @@
         <v>10.43</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>55</v>
       </c>
@@ -2898,7 +2939,7 @@
         <v>110.71</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>247</v>
       </c>
@@ -2921,7 +2962,7 @@
         <v>98.29</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>236</v>
       </c>
@@ -2944,7 +2985,7 @@
         <v>29.61</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>236</v>
       </c>
@@ -2967,7 +3008,7 @@
         <v>29.68</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>206</v>
       </c>
@@ -2990,7 +3031,7 @@
         <v>25.97</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>206</v>
       </c>
@@ -3013,7 +3054,7 @@
         <v>30.79</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>206</v>
       </c>
@@ -3036,7 +3077,7 @@
         <v>20.34</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>206</v>
       </c>
@@ -3059,7 +3100,7 @@
         <v>25.97</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>82</v>
       </c>
@@ -3082,7 +3123,7 @@
         <v>64.98</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>213</v>
       </c>
@@ -3107,13 +3148,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>